<commit_message>
🚀 Initial push of Smart Inventory & Sales System with all updates
</commit_message>
<xml_diff>
--- a/inventory_download.xlsx
+++ b/inventory_download.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J846"/>
+  <dimension ref="A1:J847"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33015,6 +33015,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Alexshirt</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="D847" t="n">
+        <v>240</v>
+      </c>
+      <c r="E847" t="n">
+        <v>180</v>
+      </c>
+      <c r="F847" t="n">
+        <v>50</v>
+      </c>
+      <c r="G847" t="inlineStr"/>
+      <c r="H847" t="inlineStr"/>
+      <c r="I847" t="n">
+        <v>0</v>
+      </c>
+      <c r="J847" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>